<commit_message>
Burndown chart efter sprint 1
</commit_message>
<xml_diff>
--- a/Sprint_backlog.xlsx
+++ b/Sprint_backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Sprint Backlog Sprint 1</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Total tid</t>
-  </si>
-  <si>
-    <t>1 timme överförs till nästa sprint</t>
   </si>
 </sst>
 </file>
@@ -133,6 +130,183 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$C$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$C$11:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="55331456"/>
+        <c:axId val="55337344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="55331456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55337344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="55337344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55331456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3752850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,12 +607,12 @@
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -455,7 +629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -475,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -495,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -515,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -529,27 +703,49 @@
         <v>4</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>